<commit_message>
import txn done and mores
</commit_message>
<xml_diff>
--- a/assets/imports/transaction_import_form_excel.xlsx
+++ b/assets/imports/transaction_import_form_excel.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t>number</t>
   </si>
@@ -49,9 +49,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>Invoice</t>
-  </si>
-  <si>
     <t>2017-12-01</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
     <t>account</t>
   </si>
   <si>
-    <t>Accounts Receivable</t>
-  </si>
-  <si>
     <t>bill_to</t>
   </si>
   <si>
@@ -100,9 +94,6 @@
     <t>tax</t>
   </si>
   <si>
-    <t>Accounts Payable</t>
-  </si>
-  <si>
     <t>INV001</t>
   </si>
   <si>
@@ -112,25 +103,10 @@
     <t>Times</t>
   </si>
   <si>
-    <t>Khmer Cake A</t>
-  </si>
-  <si>
-    <t>Khmer Cake B</t>
-  </si>
-  <si>
-    <t>INV002</t>
-  </si>
-  <si>
-    <t>Credit_Purchase</t>
-  </si>
-  <si>
     <t>Cash_Purchase</t>
   </si>
   <si>
     <t>BI001</t>
-  </si>
-  <si>
-    <t>BI002</t>
   </si>
   <si>
     <t>Cash and Cash Equivalent</t>
@@ -647,7 +623,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -655,11 +631,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -687,7 +663,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -696,10 +672,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>1</v>
@@ -708,63 +684,63 @@
         <v>6</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="O1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
         <v>15</v>
-      </c>
-      <c r="M2" t="s">
-        <v>16</v>
       </c>
       <c r="N2">
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P2">
         <v>1000</v>
@@ -773,82 +749,27 @@
         <v>1000</v>
       </c>
       <c r="R2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="L3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="N3">
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="P3">
         <v>500</v>
       </c>
       <c r="Q3">
         <v>500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>2500</v>
-      </c>
-      <c r="Q4">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="L5" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>2500</v>
-      </c>
-      <c r="Q5">
-        <v>2500</v>
       </c>
     </row>
   </sheetData>
@@ -864,11 +785,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -896,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -905,10 +826,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>1</v>
@@ -917,63 +838,63 @@
         <v>6</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="O1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
         <v>15</v>
-      </c>
-      <c r="M2" t="s">
-        <v>16</v>
       </c>
       <c r="N2">
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P2">
         <v>1000</v>
@@ -982,82 +903,27 @@
         <v>1000</v>
       </c>
       <c r="R2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="L3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="N3">
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="P3">
         <v>500</v>
       </c>
       <c r="Q3">
         <v>500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>2500</v>
-      </c>
-      <c r="Q4">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="L5" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>2500</v>
-      </c>
-      <c r="Q5">
-        <v>2500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>